<commit_message>
added new features and admin page
</commit_message>
<xml_diff>
--- a/solidworks-event/server/registrations.xlsx
+++ b/solidworks-event/server/registrations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Designation</t>
   </si>
   <si>
-    <t>Timestamp</t>
+    <t>Registered On</t>
   </si>
   <si>
     <t>Monika SM</t>
@@ -40,31 +40,13 @@
     <t>monikasm2019@gmail.com</t>
   </si>
   <si>
-    <t>Conceptia Konnect</t>
-  </si>
-  <si>
-    <t>Software developer</t>
-  </si>
-  <si>
-    <t>26/9/2025, 12:56:49 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:22:08 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:24:17 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:25:00 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:25:15 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:27:02 pm</t>
-  </si>
-  <si>
-    <t>26/9/2025, 2:28:57 pm</t>
+    <t>conceptia Konnect</t>
+  </si>
+  <si>
+    <t>Industry Solution- Expert</t>
+  </si>
+  <si>
+    <t>29/9/2025, 11:07:27 am</t>
   </si>
 </sst>
 </file>
@@ -441,12 +423,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="6" width="25" customWidth="1"/>
+    <col min="3" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -487,126 +470,6 @@
       </c>
       <c r="F2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>